<commit_message>
edit user endpoint on open API
</commit_message>
<xml_diff>
--- a/db_spesification.xlsx
+++ b/db_spesification.xlsx
@@ -403,7 +403,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -454,10 +454,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -575,13 +571,13 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>36000</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>58320</xdr:rowOff>
+      <xdr:rowOff>57960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>762840</xdr:colOff>
+      <xdr:colOff>762480</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>110880</xdr:rowOff>
+      <xdr:rowOff>110160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -590,8 +586,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="9984240" y="1944360"/>
-          <a:ext cx="726840" cy="1005120"/>
+          <a:off x="9992880" y="1943640"/>
+          <a:ext cx="726480" cy="1004760"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -631,7 +627,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>11160</xdr:colOff>
+      <xdr:colOff>10800</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>106200</xdr:rowOff>
     </xdr:to>
@@ -642,8 +638,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9948600" y="3134880"/>
-          <a:ext cx="829080" cy="360"/>
+          <a:off x="9956880" y="3134880"/>
+          <a:ext cx="829800" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -690,13 +686,13 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>1069920</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>-360</xdr:rowOff>
+      <xdr:rowOff>-720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1070280</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>170280</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -705,8 +701,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="8445960" y="3228480"/>
-          <a:ext cx="360" cy="494640"/>
+          <a:off x="8452440" y="3227760"/>
+          <a:ext cx="360" cy="494280"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -750,14 +746,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>-720</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>817920</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>93960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>10440</xdr:colOff>
+      <xdr:colOff>9360</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>94320</xdr:rowOff>
     </xdr:to>
@@ -768,8 +764,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="6557400" y="4399200"/>
-          <a:ext cx="829080" cy="360"/>
+          <a:off x="6562080" y="4399200"/>
+          <a:ext cx="829800" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -815,14 +811,14 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>1187280</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>-720</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>198720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>1187640</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>3600</xdr:rowOff>
+      <xdr:rowOff>2880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -831,8 +827,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="11953800" y="3228120"/>
-          <a:ext cx="360" cy="499680"/>
+          <a:off x="11963160" y="3227400"/>
+          <a:ext cx="360" cy="499320"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -885,7 +881,7 @@
       <xdr:col>10</xdr:col>
       <xdr:colOff>1164600</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>199080</xdr:rowOff>
+      <xdr:rowOff>198720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -894,8 +890,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="11930760" y="5297400"/>
-          <a:ext cx="360" cy="768600"/>
+          <a:off x="11940120" y="5297760"/>
+          <a:ext cx="360" cy="768240"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -940,15 +936,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>775440</xdr:colOff>
+      <xdr:colOff>775080</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>105120</xdr:rowOff>
+      <xdr:rowOff>104760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>774720</xdr:colOff>
+      <xdr:colOff>774000</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>110880</xdr:rowOff>
+      <xdr:rowOff>110160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -957,8 +953,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="9906120" y="6172560"/>
-          <a:ext cx="817200" cy="969840"/>
+          <a:off x="9912240" y="6171840"/>
+          <a:ext cx="818280" cy="969480"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -998,7 +994,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>763560</xdr:colOff>
+      <xdr:colOff>763200</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>106200</xdr:rowOff>
     </xdr:to>
@@ -1009,8 +1005,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13461840" y="6763680"/>
-          <a:ext cx="850680" cy="360"/>
+          <a:off x="13471920" y="6763680"/>
+          <a:ext cx="850320" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1057,13 +1053,13 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>975600</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>140400</xdr:rowOff>
+      <xdr:rowOff>140040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>775080</xdr:colOff>
+      <xdr:colOff>774720</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>83160</xdr:rowOff>
+      <xdr:rowOff>82440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1072,8 +1068,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="17156520" y="6207840"/>
-          <a:ext cx="836640" cy="720000"/>
+          <a:off x="17168040" y="6207120"/>
+          <a:ext cx="835560" cy="719640"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -1113,9 +1109,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>10080</xdr:colOff>
+      <xdr:colOff>9720</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>77760</xdr:rowOff>
+      <xdr:rowOff>77400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1124,8 +1120,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="13559760" y="4052160"/>
-          <a:ext cx="817200" cy="921240"/>
+          <a:off x="13569840" y="4052520"/>
+          <a:ext cx="818280" cy="920880"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -1165,9 +1161,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>775080</xdr:colOff>
+      <xdr:colOff>774720</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>92880</xdr:rowOff>
+      <xdr:rowOff>92520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1176,8 +1172,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="6557040" y="1386000"/>
-          <a:ext cx="776160" cy="2821320"/>
+          <a:off x="6560640" y="1386360"/>
+          <a:ext cx="777600" cy="2820960"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -1211,13 +1207,13 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>763200</xdr:colOff>
+      <xdr:colOff>762480</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>93600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>774360</xdr:colOff>
+      <xdr:colOff>773280</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>93960</xdr:rowOff>
     </xdr:to>
@@ -1228,8 +1224,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="3527280" y="1789200"/>
-          <a:ext cx="829080" cy="360"/>
+          <a:off x="3528000" y="1789200"/>
+          <a:ext cx="829800" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1282,7 +1278,7 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>1105560</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>163800</xdr:rowOff>
+      <xdr:rowOff>163440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1291,8 +1287,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="1923120" y="2487600"/>
-          <a:ext cx="360" cy="1228680"/>
+          <a:off x="1924200" y="2487960"/>
+          <a:ext cx="360" cy="1228320"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1339,13 +1335,13 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>1093680</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>11520</xdr:rowOff>
+      <xdr:rowOff>11160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1094040</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>10800</xdr:rowOff>
+      <xdr:rowOff>10080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1354,8 +1350,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="1911600" y="4716720"/>
-          <a:ext cx="360" cy="580320"/>
+          <a:off x="1912680" y="4716000"/>
+          <a:ext cx="360" cy="579960"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1408,7 +1404,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>976320</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>186840</xdr:rowOff>
+      <xdr:rowOff>186480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1417,8 +1413,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="5375880" y="4504320"/>
-          <a:ext cx="360" cy="768600"/>
+          <a:off x="5379840" y="4504680"/>
+          <a:ext cx="360" cy="768240"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1471,7 +1467,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>964440</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>198720</xdr:rowOff>
+      <xdr:rowOff>198360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1480,8 +1476,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="5364000" y="6078600"/>
-          <a:ext cx="360" cy="577800"/>
+          <a:off x="5367960" y="6078960"/>
+          <a:ext cx="360" cy="577440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1534,15 +1530,15 @@
   <dimension ref="A3:R44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N16" activeCellId="0" sqref="N16"/>
+      <selection pane="topLeft" activeCell="I49" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="23.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="23.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="25.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="14.69"/>
@@ -1790,10 +1786,10 @@
         <v>30</v>
       </c>
       <c r="I22" s="3"/>
-      <c r="K22" s="13" t="s">
+      <c r="K22" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="L22" s="13"/>
+      <c r="L22" s="3"/>
       <c r="N22" s="3" t="s">
         <v>32</v>
       </c>
@@ -1864,13 +1860,13 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="13" t="s">
         <v>35</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E25" s="15" t="s">
+      <c r="E25" s="14" t="s">
         <v>36</v>
       </c>
       <c r="F25" s="10" t="s">
@@ -1914,7 +1910,7 @@
       <c r="L26" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="N26" s="15" t="s">
+      <c r="N26" s="14" t="s">
         <v>14</v>
       </c>
       <c r="O26" s="10" t="s">
@@ -1928,7 +1924,7 @@
       <c r="I27" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K27" s="16" t="s">
+      <c r="K27" s="15" t="s">
         <v>44</v>
       </c>
       <c r="L27" s="5" t="s">
@@ -1942,7 +1938,7 @@
       <c r="I28" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="K28" s="16" t="s">
+      <c r="K28" s="15" t="s">
         <v>47</v>
       </c>
       <c r="L28" s="5" t="s">
@@ -1956,7 +1952,7 @@
       <c r="I29" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="K29" s="17" t="s">
+      <c r="K29" s="16" t="s">
         <v>50</v>
       </c>
       <c r="L29" s="11" t="s">
@@ -2084,7 +2080,7 @@
       <c r="O36" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="Q36" s="15" t="s">
+      <c r="Q36" s="14" t="s">
         <v>10</v>
       </c>
       <c r="R36" s="10" t="s">
@@ -2112,7 +2108,7 @@
       <c r="L37" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="N37" s="16" t="s">
+      <c r="N37" s="15" t="s">
         <v>50</v>
       </c>
       <c r="O37" s="5" t="s">
@@ -2132,7 +2128,7 @@
       <c r="F38" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H38" s="18" t="s">
+      <c r="H38" s="17" t="s">
         <v>26</v>
       </c>
       <c r="I38" s="11" t="s">
@@ -2144,7 +2140,7 @@
       <c r="L38" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="N38" s="17" t="s">
+      <c r="N38" s="16" t="s">
         <v>68</v>
       </c>
       <c r="O38" s="11" t="s">
@@ -2164,7 +2160,7 @@
       <c r="F39" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K39" s="17" t="s">
+      <c r="K39" s="16" t="s">
         <v>70</v>
       </c>
       <c r="L39" s="11" t="s">
@@ -2192,24 +2188,24 @@
       <c r="C41" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E41" s="19" t="s">
+      <c r="E41" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="F41" s="20" t="s">
+      <c r="F41" s="19" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H42" s="21"/>
-      <c r="I42" s="21"/>
+      <c r="H42" s="20"/>
+      <c r="I42" s="20"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H43" s="21"/>
-      <c r="I43" s="22"/>
+      <c r="H43" s="20"/>
+      <c r="I43" s="21"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
+      <c r="H44" s="21"/>
+      <c r="I44" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="19">

</xml_diff>